<commit_message>
Adding ABSorBEnT Data Set
</commit_message>
<xml_diff>
--- a/ABSorBEnT Data Set.xlsx
+++ b/ABSorBEnT Data Set.xlsx
@@ -11,7 +11,6 @@
     <sheet state="visible" name="Graphs" sheetId="6" r:id="rId9"/>
     <sheet state="visible" name="Tables" sheetId="7" r:id="rId10"/>
     <sheet state="visible" name="Pictures" sheetId="8" r:id="rId11"/>
-    <sheet state="hidden" name="Contents" sheetId="9" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -225,7 +224,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1913" uniqueCount="788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1877" uniqueCount="767">
   <si>
     <t>Biology</t>
   </si>
@@ -3246,69 +3245,6 @@
   <si>
     <t>TOTAL HARD</t>
   </si>
-  <si>
-    <t>TOPIC</t>
-  </si>
-  <si>
-    <t>DIFFICULTY</t>
-  </si>
-  <si>
-    <t>SUBJECT</t>
-  </si>
-  <si>
-    <t>16 categories</t>
-  </si>
-  <si>
-    <t>5 levels</t>
-  </si>
-  <si>
-    <t>3 domains</t>
-  </si>
-  <si>
-    <t>Look-up</t>
-  </si>
-  <si>
-    <t>Context-given</t>
-  </si>
-  <si>
-    <t>Comp. DNA</t>
-  </si>
-  <si>
-    <t>Easy Application</t>
-  </si>
-  <si>
-    <t>Informatics</t>
-  </si>
-  <si>
-    <t>Rev. Comp. DNA</t>
-  </si>
-  <si>
-    <t>Hard Look-up</t>
-  </si>
-  <si>
-    <t>Application</t>
-  </si>
-  <si>
-    <t>Chemical &lt;&gt; SMILES</t>
-  </si>
-  <si>
-    <t>Chemical &lt;&gt; InChI</t>
-  </si>
-  <si>
-    <t>Counting bonds</t>
-  </si>
-  <si>
-    <t>Counting atoms</t>
-  </si>
-  <si>
-    <t>Counting codons</t>
-  </si>
-  <si>
-    <t>TOTAL:</t>
-  </si>
-  <si>
-    <t>120 questions</t>
-  </si>
 </sst>
 </file>
 
@@ -3317,7 +3253,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="15">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -3400,31 +3336,6 @@
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="7.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <color theme="1"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -3532,7 +3443,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="23">
     <border/>
     <border>
       <right style="thin">
@@ -3758,83 +3669,11 @@
         <color rgb="FFFFFFFF"/>
       </top>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="124">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -4173,65 +4012,6 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="23" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="21" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="24" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="25" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="26" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="27" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="26" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="27" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="27" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="27" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="28" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="29" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="30" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="31" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="24" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="25" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="24" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="25" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="31" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -4372,11 +4152,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="280026689"/>
-        <c:axId val="562024940"/>
+        <c:axId val="941772877"/>
+        <c:axId val="1804368392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="280026689"/>
+        <c:axId val="941772877"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4428,10 +4208,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="562024940"/>
+        <c:crossAx val="1804368392"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="562024940"/>
+        <c:axId val="1804368392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.55"/>
@@ -4507,7 +4287,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="280026689"/>
+        <c:crossAx val="941772877"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -4628,11 +4408,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="918081480"/>
-        <c:axId val="1328307244"/>
+        <c:axId val="1128406341"/>
+        <c:axId val="1896967885"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="918081480"/>
+        <c:axId val="1128406341"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4684,10 +4464,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1328307244"/>
+        <c:crossAx val="1896967885"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1328307244"/>
+        <c:axId val="1896967885"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4762,7 +4542,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="918081480"/>
+        <c:crossAx val="1128406341"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -4921,11 +4701,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1298837027"/>
-        <c:axId val="1207553672"/>
+        <c:axId val="1634612470"/>
+        <c:axId val="2135485487"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1298837027"/>
+        <c:axId val="1634612470"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4977,10 +4757,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1207553672"/>
+        <c:crossAx val="2135485487"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1207553672"/>
+        <c:axId val="2135485487"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5055,7 +4835,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1298837027"/>
+        <c:crossAx val="1634612470"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -5206,11 +4986,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1881169884"/>
-        <c:axId val="1066634280"/>
+        <c:axId val="1299525491"/>
+        <c:axId val="1495995430"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1881169884"/>
+        <c:axId val="1299525491"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5262,10 +5042,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1066634280"/>
+        <c:crossAx val="1495995430"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1066634280"/>
+        <c:axId val="1495995430"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5340,7 +5120,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1881169884"/>
+        <c:crossAx val="1299525491"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -5463,11 +5243,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1315194855"/>
-        <c:axId val="397673822"/>
+        <c:axId val="746741477"/>
+        <c:axId val="1151936647"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1315194855"/>
+        <c:axId val="746741477"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5519,10 +5299,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397673822"/>
+        <c:crossAx val="1151936647"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="397673822"/>
+        <c:axId val="1151936647"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5597,7 +5377,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1315194855"/>
+        <c:crossAx val="746741477"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -5720,11 +5500,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1898023544"/>
-        <c:axId val="177474385"/>
+        <c:axId val="298559115"/>
+        <c:axId val="2131550289"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1898023544"/>
+        <c:axId val="298559115"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5776,10 +5556,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="177474385"/>
+        <c:crossAx val="2131550289"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="177474385"/>
+        <c:axId val="2131550289"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5854,7 +5634,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1898023544"/>
+        <c:crossAx val="298559115"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -5984,11 +5764,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1628427307"/>
-        <c:axId val="1022343007"/>
+        <c:axId val="725300477"/>
+        <c:axId val="256315026"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1628427307"/>
+        <c:axId val="725300477"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6040,10 +5820,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1022343007"/>
+        <c:crossAx val="256315026"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1022343007"/>
+        <c:axId val="256315026"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.55"/>
@@ -6119,7 +5899,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1628427307"/>
+        <c:crossAx val="725300477"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -6212,11 +5992,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="908852799"/>
-        <c:axId val="505423848"/>
+        <c:axId val="300577413"/>
+        <c:axId val="2074711255"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="908852799"/>
+        <c:axId val="300577413"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6268,10 +6048,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="505423848"/>
+        <c:crossAx val="2074711255"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="505423848"/>
+        <c:axId val="2074711255"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6346,7 +6126,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="908852799"/>
+        <c:crossAx val="300577413"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -6511,11 +6291,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1759584483"/>
-        <c:axId val="1572414671"/>
+        <c:axId val="1036295382"/>
+        <c:axId val="163721451"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1759584483"/>
+        <c:axId val="1036295382"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6567,10 +6347,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1572414671"/>
+        <c:crossAx val="163721451"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1572414671"/>
+        <c:axId val="163721451"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6645,7 +6425,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1759584483"/>
+        <c:crossAx val="1036295382"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -6810,11 +6590,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="2004096958"/>
-        <c:axId val="268151102"/>
+        <c:axId val="1871432087"/>
+        <c:axId val="52797579"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2004096958"/>
+        <c:axId val="1871432087"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6866,10 +6646,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="268151102"/>
+        <c:crossAx val="52797579"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="268151102"/>
+        <c:axId val="52797579"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -6945,7 +6725,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2004096958"/>
+        <c:crossAx val="1871432087"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -7110,11 +6890,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="744907726"/>
-        <c:axId val="938983970"/>
+        <c:axId val="411716243"/>
+        <c:axId val="677244986"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="744907726"/>
+        <c:axId val="411716243"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7166,10 +6946,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="938983970"/>
+        <c:crossAx val="677244986"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="938983970"/>
+        <c:axId val="677244986"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7244,7 +7024,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="744907726"/>
+        <c:crossAx val="411716243"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -7410,11 +7190,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1429232057"/>
-        <c:axId val="265450788"/>
+        <c:axId val="449319207"/>
+        <c:axId val="635941776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1429232057"/>
+        <c:axId val="449319207"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7466,10 +7246,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="265450788"/>
+        <c:crossAx val="635941776"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="265450788"/>
+        <c:axId val="635941776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7544,7 +7324,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1429232057"/>
+        <c:crossAx val="449319207"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -7702,11 +7482,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="302265798"/>
-        <c:axId val="2055969179"/>
+        <c:axId val="336812974"/>
+        <c:axId val="706556561"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="302265798"/>
+        <c:axId val="336812974"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7758,10 +7538,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2055969179"/>
+        <c:crossAx val="706556561"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2055969179"/>
+        <c:axId val="706556561"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7836,7 +7616,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302265798"/>
+        <c:crossAx val="336812974"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -7993,11 +7773,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1549144927"/>
-        <c:axId val="1877096952"/>
+        <c:axId val="1189323916"/>
+        <c:axId val="415710496"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1549144927"/>
+        <c:axId val="1189323916"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8049,10 +7829,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1877096952"/>
+        <c:crossAx val="415710496"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1877096952"/>
+        <c:axId val="415710496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8127,7 +7907,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1549144927"/>
+        <c:crossAx val="1189323916"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -8292,11 +8072,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="499173865"/>
-        <c:axId val="409733293"/>
+        <c:axId val="1542794034"/>
+        <c:axId val="1714512686"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="499173865"/>
+        <c:axId val="1542794034"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8348,10 +8128,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="409733293"/>
+        <c:crossAx val="1714512686"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="409733293"/>
+        <c:axId val="1714512686"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8426,7 +8206,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="499173865"/>
+        <c:crossAx val="1542794034"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -8591,11 +8371,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="2000348480"/>
-        <c:axId val="1319713743"/>
+        <c:axId val="720691848"/>
+        <c:axId val="1261340919"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2000348480"/>
+        <c:axId val="720691848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8647,10 +8427,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1319713743"/>
+        <c:crossAx val="1261340919"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1319713743"/>
+        <c:axId val="1261340919"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.25"/>
@@ -8726,7 +8506,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2000348480"/>
+        <c:crossAx val="720691848"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -9201,7 +8981,7 @@
     <xdr:ext cx="3829050" cy="2933700"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -9229,7 +9009,7 @@
     <xdr:ext cx="3419475" cy="2933700"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -9257,7 +9037,7 @@
     <xdr:ext cx="4133850" cy="2790825"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -9285,7 +9065,7 @@
     <xdr:ext cx="4343400" cy="2409825"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -9313,7 +9093,7 @@
     <xdr:ext cx="3905250" cy="2790825"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -9341,7 +9121,7 @@
     <xdr:ext cx="4914900" cy="2619375"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image4.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -9388,10 +9168,6 @@
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -21530,370 +21306,4 @@
   <pageSetup fitToHeight="0" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="4.25"/>
-    <col customWidth="1" min="2" max="2" width="17.75"/>
-    <col customWidth="1" min="3" max="3" width="5.88"/>
-    <col customWidth="1" min="4" max="4" width="17.75"/>
-    <col customWidth="1" min="5" max="5" width="5.88"/>
-    <col customWidth="1" min="6" max="6" width="17.75"/>
-    <col customWidth="1" min="7" max="7" width="5.88"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="124"/>
-      <c r="B1" s="124" t="s">
-        <v>767</v>
-      </c>
-      <c r="C1" s="125"/>
-      <c r="D1" s="124" t="s">
-        <v>768</v>
-      </c>
-      <c r="E1" s="125"/>
-      <c r="F1" s="124" t="s">
-        <v>769</v>
-      </c>
-      <c r="G1" s="125"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="126"/>
-      <c r="B2" s="126" t="s">
-        <v>770</v>
-      </c>
-      <c r="C2" s="127"/>
-      <c r="D2" s="126" t="s">
-        <v>771</v>
-      </c>
-      <c r="E2" s="127"/>
-      <c r="F2" s="126" t="s">
-        <v>772</v>
-      </c>
-      <c r="G2" s="127"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="128">
-        <v>1.0</v>
-      </c>
-      <c r="B3" s="129" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="130">
-        <v>5.0</v>
-      </c>
-      <c r="D3" s="129" t="s">
-        <v>773</v>
-      </c>
-      <c r="E3" s="130">
-        <v>19.0</v>
-      </c>
-      <c r="F3" s="129" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="130">
-        <v>50.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="128">
-        <v>2.0</v>
-      </c>
-      <c r="B4" s="129" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="130">
-        <v>5.0</v>
-      </c>
-      <c r="D4" s="129" t="s">
-        <v>774</v>
-      </c>
-      <c r="E4" s="130">
-        <v>6.0</v>
-      </c>
-      <c r="F4" s="129" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="130">
-        <v>37.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="128">
-        <v>3.0</v>
-      </c>
-      <c r="B5" s="129" t="s">
-        <v>775</v>
-      </c>
-      <c r="C5" s="130">
-        <v>5.0</v>
-      </c>
-      <c r="D5" s="129" t="s">
-        <v>776</v>
-      </c>
-      <c r="E5" s="130">
-        <v>2.0</v>
-      </c>
-      <c r="F5" s="129" t="s">
-        <v>777</v>
-      </c>
-      <c r="G5" s="130">
-        <v>33.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="128">
-        <v>4.0</v>
-      </c>
-      <c r="B6" s="129" t="s">
-        <v>778</v>
-      </c>
-      <c r="C6" s="130">
-        <v>5.0</v>
-      </c>
-      <c r="D6" s="129" t="s">
-        <v>779</v>
-      </c>
-      <c r="E6" s="130">
-        <v>15.0</v>
-      </c>
-      <c r="F6" s="131"/>
-      <c r="G6" s="132"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="128">
-        <v>5.0</v>
-      </c>
-      <c r="B7" s="129" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="133">
-        <v>45051.0</v>
-      </c>
-      <c r="D7" s="129" t="s">
-        <v>780</v>
-      </c>
-      <c r="E7" s="130">
-        <v>78.0</v>
-      </c>
-      <c r="F7" s="131"/>
-      <c r="G7" s="132"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="128">
-        <v>6.0</v>
-      </c>
-      <c r="B8" s="129" t="s">
-        <v>781</v>
-      </c>
-      <c r="C8" s="133">
-        <v>45051.0</v>
-      </c>
-      <c r="D8" s="131"/>
-      <c r="E8" s="132"/>
-      <c r="F8" s="131"/>
-      <c r="G8" s="132"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="128">
-        <v>7.0</v>
-      </c>
-      <c r="B9" s="129" t="s">
-        <v>782</v>
-      </c>
-      <c r="C9" s="133">
-        <v>45051.0</v>
-      </c>
-      <c r="D9" s="131"/>
-      <c r="E9" s="132"/>
-      <c r="F9" s="131"/>
-      <c r="G9" s="132"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="128">
-        <v>8.0</v>
-      </c>
-      <c r="B10" s="129" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="133">
-        <v>45051.0</v>
-      </c>
-      <c r="D10" s="131"/>
-      <c r="E10" s="132"/>
-      <c r="F10" s="131"/>
-      <c r="G10" s="132"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="128">
-        <v>9.0</v>
-      </c>
-      <c r="B11" s="129" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="133">
-        <v>45051.0</v>
-      </c>
-      <c r="D11" s="131"/>
-      <c r="E11" s="132"/>
-      <c r="F11" s="131"/>
-      <c r="G11" s="132"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="128">
-        <v>10.0</v>
-      </c>
-      <c r="B12" s="129" t="s">
-        <v>783</v>
-      </c>
-      <c r="C12" s="134" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="131"/>
-      <c r="E12" s="132"/>
-      <c r="F12" s="131"/>
-      <c r="G12" s="132"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="128">
-        <v>11.0</v>
-      </c>
-      <c r="B13" s="129" t="s">
-        <v>784</v>
-      </c>
-      <c r="C13" s="134" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="131"/>
-      <c r="E13" s="132"/>
-      <c r="F13" s="131"/>
-      <c r="G13" s="132"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="128">
-        <v>12.0</v>
-      </c>
-      <c r="B14" s="129" t="s">
-        <v>785</v>
-      </c>
-      <c r="C14" s="130">
-        <v>5.0</v>
-      </c>
-      <c r="D14" s="131"/>
-      <c r="E14" s="132"/>
-      <c r="F14" s="131"/>
-      <c r="G14" s="132"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="128">
-        <v>13.0</v>
-      </c>
-      <c r="B15" s="129" t="s">
-        <v>753</v>
-      </c>
-      <c r="C15" s="130">
-        <v>5.0</v>
-      </c>
-      <c r="D15" s="131"/>
-      <c r="E15" s="132"/>
-      <c r="F15" s="131"/>
-      <c r="G15" s="132"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="128">
-        <v>14.0</v>
-      </c>
-      <c r="B16" s="129" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="130">
-        <v>3.0</v>
-      </c>
-      <c r="D16" s="131"/>
-      <c r="E16" s="132"/>
-      <c r="F16" s="131"/>
-      <c r="G16" s="132"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="128">
-        <v>15.0</v>
-      </c>
-      <c r="B17" s="129" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="130">
-        <v>6.0</v>
-      </c>
-      <c r="D17" s="131"/>
-      <c r="E17" s="132"/>
-      <c r="F17" s="131"/>
-      <c r="G17" s="132"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="128">
-        <v>16.0</v>
-      </c>
-      <c r="B18" s="129" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="130">
-        <v>4.0</v>
-      </c>
-      <c r="D18" s="131"/>
-      <c r="E18" s="132"/>
-      <c r="F18" s="131"/>
-      <c r="G18" s="132"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="128"/>
-      <c r="B19" s="129"/>
-      <c r="C19" s="130"/>
-      <c r="D19" s="131"/>
-      <c r="E19" s="132"/>
-      <c r="G19" s="132"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="135"/>
-      <c r="B20" s="131"/>
-      <c r="C20" s="132"/>
-      <c r="D20" s="136" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" s="137">
-        <f>sum(E3:E6)</f>
-        <v>42</v>
-      </c>
-      <c r="F20" s="138" t="s">
-        <v>786</v>
-      </c>
-      <c r="G20" s="137"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="139"/>
-      <c r="B21" s="140"/>
-      <c r="C21" s="141"/>
-      <c r="D21" s="142" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="143">
-        <f>E7</f>
-        <v>78</v>
-      </c>
-      <c r="F21" s="144" t="s">
-        <v>787</v>
-      </c>
-      <c r="G21" s="141"/>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>